<commit_message>
Werkelijk resultaat toegevoegd aan werkbestand zodat syncen nu goed gaat
</commit_message>
<xml_diff>
--- a/Werkbestand Projectadministratie.xlsx
+++ b/Werkbestand Projectadministratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3F4565-327C-46B2-9875-D6B54F9AD7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE29B95-F108-44BB-904C-465BBD824764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,43 +44,43 @@
     <t xml:space="preserve">Algemene informatie </t>
   </si>
   <si>
+    <t>Omschrijving</t>
+  </si>
+  <si>
+    <t>Actiepunten Projectleider</t>
+  </si>
+  <si>
+    <t>Projectleider</t>
+  </si>
+  <si>
+    <t>Klant</t>
+  </si>
+  <si>
+    <t>Aangepast resultaat</t>
+  </si>
+  <si>
+    <t>Actiepunten Bram</t>
+  </si>
+  <si>
+    <t>Bespreekpunten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum: </t>
+  </si>
+  <si>
+    <t>Whitelist</t>
+  </si>
+  <si>
+    <t>Actiepunten Elders</t>
+  </si>
+  <si>
+    <t>2e Projectleider</t>
+  </si>
+  <si>
+    <t>Werkelijk resultaat</t>
+  </si>
+  <si>
     <t>Verwacht resultaat</t>
-  </si>
-  <si>
-    <t>Omschrijving</t>
-  </si>
-  <si>
-    <t>Actiepunten Projectleider</t>
-  </si>
-  <si>
-    <t>Projectleider</t>
-  </si>
-  <si>
-    <t>Klant</t>
-  </si>
-  <si>
-    <t>Aangepast resultaat</t>
-  </si>
-  <si>
-    <t>Actiepunten Bram</t>
-  </si>
-  <si>
-    <t>Bespreekpunten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum: </t>
-  </si>
-  <si>
-    <t>Whitelist</t>
-  </si>
-  <si>
-    <t>Actiepunten Elders</t>
-  </si>
-  <si>
-    <t>2e Projectleider</t>
-  </si>
-  <si>
-    <t>Werkelijk resultaat</t>
   </si>
 </sst>
 </file>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -146,9 +146,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -432,14 +429,14 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="5" width="17.77734375" customWidth="1"/>
-    <col min="6" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.5546875" customWidth="1"/>
     <col min="9" max="11" width="25.77734375" customWidth="1"/>
     <col min="12" max="12" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
@@ -448,7 +445,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -469,43 +466,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created an overview in another sheet within werkbestand for me to easily work on closing project
</commit_message>
<xml_diff>
--- a/Werkbestand Projectadministratie.xlsx
+++ b/Werkbestand Projectadministratie.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram.gerrits\Desktop\Automations\ProjectAdministration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CA5A32-3E5C-4D5C-8AB6-61B5F746E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACA6205-AC9C-40D5-8B7F-B97AF658235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Projecten Afsluiten" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,30 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Project</t>
   </si>
@@ -104,6 +82,9 @@
   </si>
   <si>
     <t>Verwacht resultaat</t>
+  </si>
+  <si>
+    <t>Projectnummer</t>
   </si>
 </sst>
 </file>
@@ -452,7 +433,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,10 +516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AED606-DE23-40D2-92AD-E6B1C9E4B982}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +533,7 @@
       </c>
       <c r="B1" s="1" t="str">
         <f ca="1">"Datum: "&amp;TEXT(NOW(),"dd-mm-jjjj")</f>
-        <v>Datum: 24-10-2025</v>
+        <v>Datum: 30-10-2025</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -560,7 +541,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -573,25 +554,6 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="str" cm="1">
-        <f t="array" aca="1" ref="A3" ca="1">_xlfn.LET(
-  _xlpm.Hdrs, Sheet1!$A$2:$Z$2,
-  _xlpm.Data, Sheet1!$A$3:$Z$9999,
-  _xlpm.iAPB, MATCH("Actiepunten Bram", _xlpm.Hdrs, 0),
-  _xlpm.Cond, BYRY(_xlpm.Data,,_xlpm.iAPB,
-        _xlfn.LAMBDA(_xlpm.c, _xlfn.LET(
-          _xlpm.t, LAGER(_xlpm.c),
-          SUM(--ISNUMBER(LOOKUP({"sluit";"afsluit";"afsluiten";"sluiten";"afronden";"afrond"}, _xlpm.t)))&gt;0
-        ))
-      ),
-  _xlpm.Rijen, _xlfn._xlws.FILTER(_xlpm.Data, _xlpm.Cond),
-  _xlpm.Kolommen, MATCH({"Project";"Projectleider";"Klant";"Omschrijving";"Actiepunten Bram"}, _xlpm.Hdrs, 0),
-  IFERROR(KIESKOLOMMEN(_xlpm.Rijen, _xlpm.Kolommen), "— Geen projecten gevonden —")
-)</f>
-        <v>— Geen projecten gevonden —</v>
       </c>
     </row>
   </sheetData>

</xml_diff>